<commit_message>
modificato formula media e somma
</commit_message>
<xml_diff>
--- a/Week4/Day1/Day1-excel-schillaci.xlsx
+++ b/Week4/Day1/Day1-excel-schillaci.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giuseppe/Documents/GitHub/epicode-data-analyst/Week4/Day1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC21CD1-B050-BD47-B196-AA28B9207D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C411B76B-BE4B-014D-8D52-5682B49FBA59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{06F27914-2FA5-6743-A1C9-BF26F1409FA6}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="16340" xr2:uid="{06F27914-2FA5-6743-A1C9-BF26F1409FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sol-Esercizio1-giorni" sheetId="2" r:id="rId1"/>
@@ -915,7 +915,7 @@
   <dimension ref="A2:U17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -976,11 +976,11 @@
         <v>2300</v>
       </c>
       <c r="G3" s="11">
-        <f>SUM(C3:E3)</f>
+        <f>C3+D3+E3</f>
         <v>8470</v>
       </c>
       <c r="H3" s="11">
-        <f>AVERAGE(C3:E3)</f>
+        <f>G3/3</f>
         <v>2823.3333333333335</v>
       </c>
     </row>
@@ -998,11 +998,11 @@
         <v>2600</v>
       </c>
       <c r="G4" s="11">
-        <f t="shared" ref="G4:G7" si="0">SUM(C4:E4)</f>
+        <f t="shared" ref="G4:G14" si="0">C4+D4+E4</f>
         <v>8260</v>
       </c>
       <c r="H4" s="11">
-        <f t="shared" ref="H4:H6" si="1">AVERAGE(C4:E4)</f>
+        <f t="shared" ref="H4:H14" si="1">G4/3</f>
         <v>2753.3333333333335</v>
       </c>
     </row>
@@ -1068,7 +1068,7 @@
         <v>8161</v>
       </c>
       <c r="H7" s="11">
-        <f>AVERAGE(C7:E7)</f>
+        <f t="shared" si="1"/>
         <v>2720.3333333333335</v>
       </c>
     </row>

</xml_diff>